<commit_message>
finished tasks 1, 2 and 3
</commit_message>
<xml_diff>
--- a/MGMT220_ShortSurvey_2016.xlsx
+++ b/MGMT220_ShortSurvey_2016.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xeton\Desktop\Macquarie Uni\MGMT220\MGMT220\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCD99652-7FC8-4699-B519-CA5F0F65A449}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3D545048-6DA2-4DFD-9DC2-F133CE3DECE2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
     <sheet name="DataTable" sheetId="1" r:id="rId2"/>
     <sheet name="Functions" sheetId="3" r:id="rId3"/>
+    <sheet name="DataPlay" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="Challenging">DataPlay!$G$1:$G$31</definedName>
+    <definedName name="GainSkills">DataPlay!$I$1:$I$31</definedName>
+    <definedName name="Worthwhile">DataPlay!$H$1:$H$31</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -378,6 +384,21 @@
   </si>
   <si>
     <t>Commerce/Business</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>StDev</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q3</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2248,7 +2269,7 @@
       </c>
       <c r="C24" s="12" t="str">
         <f ca="1">TEXT(WEEKDAY(NOW()),"dddd")</f>
-        <v>Friday</v>
+        <v>Tuesday</v>
       </c>
       <c r="D24" s="18"/>
     </row>
@@ -2326,4 +2347,988 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76D4C0E-CFCC-40A3-BF82-0AF756C70F6F}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
+    <col min="6" max="9" width="11.5703125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>5</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>7</v>
+      </c>
+      <c r="H20" s="1">
+        <v>7</v>
+      </c>
+      <c r="I20" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5</v>
+      </c>
+      <c r="H21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4</v>
+      </c>
+      <c r="I26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1">
+        <v>5</v>
+      </c>
+      <c r="H27" s="1">
+        <v>6</v>
+      </c>
+      <c r="I27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4</v>
+      </c>
+      <c r="G28" s="1">
+        <v>5</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>4</v>
+      </c>
+      <c r="H29" s="1">
+        <v>5</v>
+      </c>
+      <c r="I29" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>7</v>
+      </c>
+      <c r="H30" s="1">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="18">
+        <f>AVERAGE($F$2:$F$31)</f>
+        <v>3.7333333333333334</v>
+      </c>
+      <c r="G33" s="18">
+        <f>AVERAGE(Challenging)</f>
+        <v>4.4333333333333336</v>
+      </c>
+      <c r="H33" s="18">
+        <f>AVERAGE(Worthwhile)</f>
+        <v>4.4137931034482758</v>
+      </c>
+      <c r="I33" s="1">
+        <f>AVERAGE(GainSkills)</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="18">
+        <f>_xlfn.STDEV.S($F$2:$F$31)</f>
+        <v>1.1724814044061258</v>
+      </c>
+      <c r="G34" s="18">
+        <f>_xlfn.STDEV.S(Challenging)</f>
+        <v>1.4064710873459967</v>
+      </c>
+      <c r="H34" s="18">
+        <f>_xlfn.STDEV.S(Worthwhile)</f>
+        <v>1.3500592944467913</v>
+      </c>
+      <c r="I34" s="1">
+        <f>_xlfn.STDEV.S(GainSkills)</f>
+        <v>1.2056963563450391</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="18">
+        <f>MEDIAN($F$2:$F$31)</f>
+        <v>4</v>
+      </c>
+      <c r="G35" s="18">
+        <f>MEDIAN(Challenging)</f>
+        <v>4</v>
+      </c>
+      <c r="H35" s="18">
+        <f>MEDIAN(Worthwhile)</f>
+        <v>4</v>
+      </c>
+      <c r="I35" s="1">
+        <f>MEDIAN(GainSkills)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="18">
+        <f>_xlfn.QUARTILE.EXC($F$2:$F$31, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="G36" s="18">
+        <f>_xlfn.QUARTILE.EXC(Challenging, 1)</f>
+        <v>3.75</v>
+      </c>
+      <c r="H36" s="18">
+        <f>_xlfn.QUARTILE.EXC(Worthwhile, 1)</f>
+        <v>3.5</v>
+      </c>
+      <c r="I36" s="1">
+        <f>_xlfn.QUARTILE.EXC(GainSkills, 1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="18">
+        <f>_xlfn.QUARTILE.EXC($F$2:$F$31, 3)</f>
+        <v>5</v>
+      </c>
+      <c r="G37" s="18">
+        <f>_xlfn.QUARTILE.EXC(Challenging, 3)</f>
+        <v>5</v>
+      </c>
+      <c r="H37" s="18">
+        <f>_xlfn.QUARTILE.EXC(Worthwhile, 3)</f>
+        <v>5.5</v>
+      </c>
+      <c r="I37" s="1">
+        <f>_xlfn.QUARTILE.EXC(GainSkills, 3)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started Task 4 and should note the file is not the same as the instructions
</commit_message>
<xml_diff>
--- a/MGMT220_ShortSurvey_2016.xlsx
+++ b/MGMT220_ShortSurvey_2016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xeton\Desktop\Macquarie Uni\MGMT220\MGMT220\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3D545048-6DA2-4DFD-9DC2-F133CE3DECE2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B7B572E6-B3F4-40F7-AE5F-5E34AB9611D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,10 @@
   </sheets>
   <definedNames>
     <definedName name="Challenging">DataPlay!$G$1:$G$31</definedName>
+    <definedName name="elective">DataPlay!$C$2:$C$31</definedName>
     <definedName name="GainSkills">DataPlay!$I$1:$I$31</definedName>
+    <definedName name="program">DataPlay!$D$2:$D$31</definedName>
+    <definedName name="Sex">DataPlay!$E$2:$E$31</definedName>
     <definedName name="Worthwhile">DataPlay!$H$1:$H$31</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -2353,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76D4C0E-CFCC-40A3-BF82-0AF756C70F6F}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3222,7 +3225,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <f>COUNT($C$2:$C$31)</f>
+        <v>22</v>
+      </c>
+      <c r="D33" s="1">
+        <f>COUNT($D$2:$D$31)</f>
+        <v>26</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>117</v>
       </c>
@@ -3238,12 +3249,12 @@
         <f>AVERAGE(Worthwhile)</f>
         <v>4.4137931034482758</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="18">
         <f>AVERAGE(GainSkills)</f>
         <v>4.25</v>
       </c>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
         <v>118</v>
       </c>
@@ -3259,12 +3270,12 @@
         <f>_xlfn.STDEV.S(Worthwhile)</f>
         <v>1.3500592944467913</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="18">
         <f>_xlfn.STDEV.S(GainSkills)</f>
         <v>1.2056963563450391</v>
       </c>
     </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
         <v>119</v>
       </c>
@@ -3280,12 +3291,12 @@
         <f>MEDIAN(Worthwhile)</f>
         <v>4</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="18">
         <f>MEDIAN(GainSkills)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
         <v>120</v>
       </c>
@@ -3301,12 +3312,12 @@
         <f>_xlfn.QUARTILE.EXC(Worthwhile, 1)</f>
         <v>3.5</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="18">
         <f>_xlfn.QUARTILE.EXC(GainSkills, 1)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="s">
         <v>121</v>
       </c>
@@ -3322,7 +3333,7 @@
         <f>_xlfn.QUARTILE.EXC(Worthwhile, 3)</f>
         <v>5.5</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="18">
         <f>_xlfn.QUARTILE.EXC(GainSkills, 3)</f>
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
finished practical 2 exercises
</commit_message>
<xml_diff>
--- a/MGMT220_ShortSurvey_2016.xlsx
+++ b/MGMT220_ShortSurvey_2016.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xeton\Desktop\Macquarie Uni\MGMT220\MGMT220\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howde\Documents\Repos\MGMT220\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B7B572E6-B3F4-40F7-AE5F-5E34AB9611D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943CC3D-512C-4F20-B945-00845B7DA435}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,16 @@
     <sheet name="DataPlay" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Challenging">DataPlay!$G$1:$G$31</definedName>
+    <definedName name="Challenging">DataPlay!$H$1:$H$31</definedName>
     <definedName name="elective">DataPlay!$C$2:$C$31</definedName>
-    <definedName name="GainSkills">DataPlay!$I$1:$I$31</definedName>
+    <definedName name="ElectiveLabels">Notes!$A$15:$B$17</definedName>
+    <definedName name="GainSkills">DataPlay!$J$1:$J$31</definedName>
     <definedName name="program">DataPlay!$D$2:$D$31</definedName>
+    <definedName name="ProgramLabels">Notes!$A$4:$B$9</definedName>
     <definedName name="Sex">DataPlay!$E$2:$E$31</definedName>
-    <definedName name="Worthwhile">DataPlay!$H$1:$H$31</definedName>
+    <definedName name="Worthwhile">DataPlay!$I$1:$I$31</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="125">
   <si>
     <t>ID</t>
   </si>
@@ -402,6 +404,15 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>SexL</t>
+  </si>
+  <si>
+    <t>ProgramL</t>
+  </si>
+  <si>
+    <t>ElectiveL</t>
   </si>
 </sst>
 </file>
@@ -944,17 +955,17 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A15" sqref="A15:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="8" width="16.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.59765625" style="1" customWidth="1"/>
+    <col min="2" max="8" width="16.1328125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -966,7 +977,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>40</v>
       </c>
@@ -980,7 +991,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -992,7 +1003,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="7" t="s">
         <v>43</v>
       </c>
@@ -1006,7 +1017,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1020,7 +1031,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1032,7 +1043,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -1044,7 +1055,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1056,7 +1067,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -1068,7 +1079,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="E10" s="4"/>
@@ -1076,7 +1087,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
@@ -1084,7 +1095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -1092,7 +1103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -1100,11 +1111,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="7" t="s">
         <v>53</v>
       </c>
@@ -1112,7 +1123,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="8">
         <v>2</v>
       </c>
@@ -1128,12 +1139,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="9" t="s">
         <v>5</v>
       </c>
@@ -1147,12 +1158,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1178,7 +1189,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
@@ -1223,18 +1234,18 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
-    <col min="6" max="9" width="11.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" style="1" customWidth="1"/>
+    <col min="6" max="9" width="11.59765625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1263,7 +1274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1292,7 +1303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1321,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1347,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1376,7 +1387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1405,7 +1416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1434,7 +1445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1457,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1486,7 +1497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1515,7 +1526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1544,7 +1555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1573,7 +1584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1602,7 +1613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1631,7 +1642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1660,7 +1671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1686,7 +1697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1715,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1744,7 +1755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1773,7 +1784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1802,7 +1813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1828,7 +1839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1854,7 +1865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1880,7 +1891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1906,7 +1917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1929,7 +1940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1958,7 +1969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1987,7 +1998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2010,7 +2021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2039,7 +2050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2062,7 +2073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2101,16 +2112,16 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="21.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>68</v>
       </c>
@@ -2118,7 +2129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" s="12" t="s">
         <v>70</v>
       </c>
@@ -2126,19 +2137,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" s="12"/>
       <c r="B3" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" s="13" t="s">
         <v>74</v>
       </c>
@@ -2146,19 +2157,19 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" s="13"/>
       <c r="B7" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8" s="14" t="s">
         <v>78</v>
       </c>
@@ -2166,19 +2177,19 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10" s="14"/>
       <c r="B10" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A11" s="15" t="s">
         <v>82</v>
       </c>
@@ -2186,25 +2197,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" s="15"/>
       <c r="B12" s="15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A13" s="15"/>
       <c r="B13" s="15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" s="16" t="s">
         <v>87</v>
       </c>
@@ -2212,25 +2223,25 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" s="16"/>
       <c r="B16" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="16"/>
       <c r="B18" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" s="14" t="s">
         <v>92</v>
       </c>
@@ -2238,32 +2249,32 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="14"/>
       <c r="B21" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="14"/>
       <c r="B23" s="14" t="s">
         <v>97</v>
       </c>
       <c r="C23" s="17"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="12" t="s">
         <v>98</v>
       </c>
@@ -2272,11 +2283,11 @@
       </c>
       <c r="C24" s="12" t="str">
         <f ca="1">TEXT(WEEKDAY(NOW()),"dddd")</f>
-        <v>Tuesday</v>
+        <v>Wednesday</v>
       </c>
       <c r="D24" s="18"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" s="13" t="s">
         <v>100</v>
       </c>
@@ -2287,7 +2298,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="19" t="s">
         <v>103</v>
       </c>
@@ -2295,31 +2306,31 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" s="19"/>
       <c r="B27" s="19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="19"/>
       <c r="B28" s="19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="19"/>
       <c r="B29" s="19" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="19"/>
       <c r="B30" s="19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="15" t="s">
         <v>109</v>
       </c>
@@ -2327,19 +2338,19 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="15"/>
       <c r="B32" s="15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A33" s="15"/>
       <c r="B33" s="15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A34" s="14" t="s">
         <v>113</v>
       </c>
@@ -2354,24 +2365,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76D4C0E-CFCC-40A3-BF82-0AF756C70F6F}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33:I37"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="9" width="11.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="7.86328125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="11.59765625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" style="1"/>
+    <col min="12" max="12" width="17" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.53125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2387,20 +2401,30 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2416,20 +2440,32 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
       <c r="G2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
         <v>6</v>
       </c>
-      <c r="I2" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>VLOOKUP(E2,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L2" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D2, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C2, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2445,20 +2481,32 @@
       <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
-        <v>5</v>
-      </c>
       <c r="G3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>VLOOKUP(E3,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D3, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Economics</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C3, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2471,20 +2519,32 @@
       <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
       <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
         <v>6</v>
       </c>
-      <c r="H4" s="1">
-        <v>5</v>
-      </c>
       <c r="I4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f>VLOOKUP(E4,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D4, ProgramLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C4, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2500,20 +2560,32 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>6</v>
       </c>
-      <c r="G5" s="1">
-        <v>4</v>
-      </c>
       <c r="H5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>VLOOKUP(E5,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D5, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C5, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2529,20 +2601,32 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
       <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
         <v>6</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>7</v>
       </c>
-      <c r="I6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f>VLOOKUP(E6,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D6, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Science</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C6, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2558,20 +2642,32 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
-        <v>4</v>
-      </c>
       <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
         <v>7</v>
-      </c>
-      <c r="H7" s="1">
-        <v>6</v>
       </c>
       <c r="I7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f>VLOOKUP(E7,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D7, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C7, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2584,17 +2680,29 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
-        <v>5</v>
-      </c>
       <c r="G8" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f>VLOOKUP(E8,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D8, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C8, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2610,20 +2718,32 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="1">
-        <v>4</v>
-      </c>
       <c r="G9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f>VLOOKUP(E9,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D9, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C9, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2639,20 +2759,32 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
-        <v>3</v>
-      </c>
       <c r="G10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f>VLOOKUP(E10,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D10, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C10, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2668,20 +2800,32 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="1">
-        <v>5</v>
-      </c>
       <c r="G11" s="1">
         <v>5</v>
       </c>
       <c r="H11" s="1">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="str">
+        <f>VLOOKUP(E11,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L11" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D11, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C11, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2697,20 +2841,32 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
       <c r="G12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12" s="1">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="str">
+        <f>VLOOKUP(E12,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L12" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D12, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Arts</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C12, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2726,20 +2882,32 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="1">
-        <v>5</v>
-      </c>
       <c r="G13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1">
         <v>4</v>
       </c>
       <c r="I13" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f>VLOOKUP(E13,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L13" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D13, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C13, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2755,20 +2923,32 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="1">
-        <v>5</v>
-      </c>
       <c r="G14" s="1">
         <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f>VLOOKUP(E14,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L14" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D14, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C14, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2784,20 +2964,32 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="1">
-        <v>5</v>
-      </c>
       <c r="G15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f>VLOOKUP(E15,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L15" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D15, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M15" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C15, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2810,20 +3002,32 @@
       <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
       <c r="G16" s="1">
         <v>4</v>
       </c>
       <c r="H16" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f>VLOOKUP(E16,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L16" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D16, ProgramLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+      <c r="M16" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C16, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2839,20 +3043,32 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="1">
-        <v>5</v>
-      </c>
       <c r="G17" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f>VLOOKUP(E17,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L17" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D17, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M17" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C17, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2868,20 +3084,32 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
       <c r="G18" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1">
+        <v>4</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f>VLOOKUP(E18,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L18" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D18, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C18, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2897,20 +3125,32 @@
       <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="1">
-        <v>4</v>
-      </c>
       <c r="G19" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1">
+        <v>5</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f>VLOOKUP(E19,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L19" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D19, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M19" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C19, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2926,20 +3166,32 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="1">
-        <v>3</v>
-      </c>
       <c r="G20" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H20" s="1">
         <v>7</v>
       </c>
       <c r="I20" s="1">
+        <v>7</v>
+      </c>
+      <c r="J20" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="str">
+        <f>VLOOKUP(E20,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L20" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D20, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M20" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C20, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2952,20 +3204,32 @@
       <c r="E21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="1">
-        <v>4</v>
-      </c>
       <c r="G21" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f>VLOOKUP(E21,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L21" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D21, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M21" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C21, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2978,20 +3242,32 @@
       <c r="E22" s="1">
         <v>1</v>
       </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
       <c r="G22" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I22" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1">
+        <v>4</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f>VLOOKUP(E22,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L22" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D22, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C22, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3004,20 +3280,32 @@
       <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="F23" s="1">
-        <v>3</v>
-      </c>
       <c r="G23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f>VLOOKUP(E23,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L23" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D23, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M23" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C23, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3030,20 +3318,32 @@
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="1">
-        <v>4</v>
-      </c>
       <c r="G24" s="1">
         <v>4</v>
       </c>
       <c r="H24" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I24" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1">
+        <v>3</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f>VLOOKUP(E24,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L24" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D24, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C24, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3056,17 +3356,29 @@
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
       <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
         <v>6</v>
       </c>
-      <c r="H25" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="1">
+        <v>5</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f>VLOOKUP(E25,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L25" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D25, ProgramLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C25, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3082,9 +3394,6 @@
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="1">
-        <v>4</v>
-      </c>
       <c r="G26" s="1">
         <v>4</v>
       </c>
@@ -3092,10 +3401,25 @@
         <v>4</v>
       </c>
       <c r="I26" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1">
+        <v>5</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f>VLOOKUP(E26,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L26" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D26, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C26, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3111,20 +3435,32 @@
       <c r="E27" s="1">
         <v>2</v>
       </c>
-      <c r="F27" s="1">
-        <v>4</v>
-      </c>
       <c r="G27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H27" s="1">
+        <v>5</v>
+      </c>
+      <c r="I27" s="1">
         <v>6</v>
       </c>
-      <c r="I27" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1">
+        <v>5</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f>VLOOKUP(E27,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L27" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D27, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C27, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Elective</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3137,17 +3473,29 @@
       <c r="E28" s="1">
         <v>2</v>
       </c>
-      <c r="F28" s="1">
-        <v>4</v>
-      </c>
       <c r="G28" s="1">
-        <v>5</v>
-      </c>
-      <c r="I28" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f>VLOOKUP(E28,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L28" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D28, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M28" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C28, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3163,20 +3511,32 @@
       <c r="E29" s="1">
         <v>2</v>
       </c>
-      <c r="F29" s="1">
-        <v>3</v>
-      </c>
       <c r="G29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H29" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J29" s="1">
+        <v>4</v>
+      </c>
+      <c r="K29" s="1" t="str">
+        <f>VLOOKUP(E29,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L29" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D29, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Business Analytics</v>
+      </c>
+      <c r="M29" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C29, ElectiveLabels, 2, FALSE),  "")</f>
+        <v>Compulsory</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3186,20 +3546,32 @@
       <c r="E30" s="1">
         <v>2</v>
       </c>
-      <c r="F30" s="1">
-        <v>4</v>
-      </c>
       <c r="G30" s="1">
+        <v>4</v>
+      </c>
+      <c r="H30" s="1">
         <v>7</v>
-      </c>
-      <c r="H30" s="1">
-        <v>6</v>
       </c>
       <c r="I30" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="1">
+        <v>6</v>
+      </c>
+      <c r="K30" s="1" t="str">
+        <f>VLOOKUP(E30,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Female</v>
+      </c>
+      <c r="L30" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D30, ProgramLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+      <c r="M30" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C30, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3212,20 +3584,32 @@
       <c r="E31" s="1">
         <v>1</v>
       </c>
-      <c r="F31" s="1">
-        <v>3</v>
-      </c>
       <c r="G31" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H31" s="1">
         <v>4</v>
       </c>
       <c r="I31" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J31" s="1">
+        <v>3</v>
+      </c>
+      <c r="K31" s="1" t="str">
+        <f>VLOOKUP(E31,Notes!$A$12:$B$13, 2, FALSE)</f>
+        <v>Male</v>
+      </c>
+      <c r="L31" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(D31, ProgramLabels, 2, FALSE),  "")</f>
+        <v>Commerce/Business</v>
+      </c>
+      <c r="M31" s="1" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C31, ElectiveLabels, 2, FALSE),  "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.5">
       <c r="C33" s="1">
         <f>COUNT($C$2:$C$31)</f>
         <v>22</v>
@@ -3234,112 +3618,124 @@
         <f>COUNT($D$2:$D$31)</f>
         <v>26</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="1">
+        <f>COUNT(Sex)</f>
+        <v>30</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="18">
-        <f>AVERAGE($F$2:$F$31)</f>
+      <c r="G33" s="18">
+        <f>AVERAGE($G$2:$G$31)</f>
         <v>3.7333333333333334</v>
       </c>
-      <c r="G33" s="18">
+      <c r="H33" s="18">
         <f>AVERAGE(Challenging)</f>
         <v>4.4333333333333336</v>
       </c>
-      <c r="H33" s="18">
+      <c r="I33" s="18">
         <f>AVERAGE(Worthwhile)</f>
         <v>4.4137931034482758</v>
       </c>
-      <c r="I33" s="18">
+      <c r="J33" s="18">
         <f>AVERAGE(GainSkills)</f>
         <v>4.25</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="1" t="s">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.5">
+      <c r="F34" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="18">
-        <f>_xlfn.STDEV.S($F$2:$F$31)</f>
+      <c r="G34" s="18">
+        <f>_xlfn.STDEV.S($G$2:$G$31)</f>
         <v>1.1724814044061258</v>
       </c>
-      <c r="G34" s="18">
+      <c r="H34" s="18">
         <f>_xlfn.STDEV.S(Challenging)</f>
         <v>1.4064710873459967</v>
       </c>
-      <c r="H34" s="18">
+      <c r="I34" s="18">
         <f>_xlfn.STDEV.S(Worthwhile)</f>
         <v>1.3500592944467913</v>
       </c>
-      <c r="I34" s="18">
+      <c r="J34" s="18">
         <f>_xlfn.STDEV.S(GainSkills)</f>
         <v>1.2056963563450391</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="1" t="s">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.5">
+      <c r="E35" s="1">
+        <f>COUNTIF(Sex, 1)</f>
+        <v>16</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F35" s="18">
-        <f>MEDIAN($F$2:$F$31)</f>
-        <v>4</v>
-      </c>
       <c r="G35" s="18">
+        <f>MEDIAN($G$2:$G$31)</f>
+        <v>4</v>
+      </c>
+      <c r="H35" s="18">
         <f>MEDIAN(Challenging)</f>
         <v>4</v>
       </c>
-      <c r="H35" s="18">
+      <c r="I35" s="18">
         <f>MEDIAN(Worthwhile)</f>
         <v>4</v>
       </c>
-      <c r="I35" s="18">
+      <c r="J35" s="18">
         <f>MEDIAN(GainSkills)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E36" s="1" t="s">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.5">
+      <c r="E36" s="1">
+        <f>COUNTIF(Sex, 2)</f>
+        <v>14</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="18">
-        <f>_xlfn.QUARTILE.EXC($F$2:$F$31, 1)</f>
-        <v>3</v>
-      </c>
       <c r="G36" s="18">
+        <f>_xlfn.QUARTILE.EXC($G$2:$G$31, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="H36" s="18">
         <f>_xlfn.QUARTILE.EXC(Challenging, 1)</f>
         <v>3.75</v>
       </c>
-      <c r="H36" s="18">
+      <c r="I36" s="18">
         <f>_xlfn.QUARTILE.EXC(Worthwhile, 1)</f>
         <v>3.5</v>
       </c>
-      <c r="I36" s="18">
+      <c r="J36" s="18">
         <f>_xlfn.QUARTILE.EXC(GainSkills, 1)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E37" s="1" t="s">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.5">
+      <c r="F37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F37" s="18">
-        <f>_xlfn.QUARTILE.EXC($F$2:$F$31, 3)</f>
-        <v>5</v>
-      </c>
       <c r="G37" s="18">
+        <f>_xlfn.QUARTILE.EXC($G$2:$G$31, 3)</f>
+        <v>5</v>
+      </c>
+      <c r="H37" s="18">
         <f>_xlfn.QUARTILE.EXC(Challenging, 3)</f>
         <v>5</v>
       </c>
-      <c r="H37" s="18">
+      <c r="I37" s="18">
         <f>_xlfn.QUARTILE.EXC(Worthwhile, 3)</f>
         <v>5.5</v>
       </c>
-      <c r="I37" s="18">
+      <c r="J37" s="18">
         <f>_xlfn.QUARTILE.EXC(GainSkills, 3)</f>
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>